<commit_message>
Petit 4 and others
</commit_message>
<xml_diff>
--- a/databases/Orcus - Feats.xlsx
+++ b/databases/Orcus - Feats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Obsidian\Tabletop games\d20 System or D&amp;D-esque\2021 Orcus - 4E clone\GitHub\orcus\databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31164E04-1A10-44F7-AE29-7BEBDC03EB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7A270A-5717-4BDB-8480-A5394D4A8DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="229">
   <si>
     <t># Shard Feats</t>
   </si>
@@ -703,6 +703,27 @@
   </si>
   <si>
     <t>You gain access to the **psi focus** power. You do not have any focus surges.</t>
+  </si>
+  <si>
+    <t>Improved Maneuver</t>
+  </si>
+  <si>
+    <t>You do not provoke  attacks of opportunity when you use the *disarm, trip, sunder* or *overrun* powers.</t>
+  </si>
+  <si>
+    <t>Advanced Combat</t>
+  </si>
+  <si>
+    <t>Flicking Disarm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you *disarm* a target, you can choose any unoccupied square adjacent to you or the target for the item to land in. </t>
+  </si>
+  <si>
+    <t>Distant Maneuver</t>
+  </si>
+  <si>
+    <t>You can *disarm, trip* or *sunder* using a ranged weapon.</t>
   </si>
 </sst>
 </file>
@@ -1034,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2059,8 +2080,50 @@
       <c r="A59" s="1" t="s">
         <v>200</v>
       </c>
+      <c r="B59" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="E59" s="1" t="s">
         <v>221</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>